<commit_message>
[VSW][APP] Make Localization #21 [ISSUE] VSW # 21 [DES] Part_1
</commit_message>
<xml_diff>
--- a/Document/Localization.xlsx
+++ b/Document/Localization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -728,21 +728,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -821,11 +812,102 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="45">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -853,6 +935,29 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -865,84 +970,9 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -972,34 +1002,249 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1019,7 +1264,21 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1039,7 +1298,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1073,41 +1332,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1176,6 +1401,26 @@
         </patternFill>
       </fill>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1310,111 +1555,17 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -1447,6 +1598,43 @@
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1464,7 +1652,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1498,7 +1686,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1532,7 +1720,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1590,17 +1778,17 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="13"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1622,194 +1810,6 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1824,78 +1824,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D13" totalsRowShown="0" headerRowDxfId="44" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D13" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A4:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="STT" dataDxfId="13"/>
-    <tableColumn id="2" name="ID" dataDxfId="12"/>
-    <tableColumn id="3" name="Text Vietnameses" dataDxfId="11"/>
-    <tableColumn id="4" name="Text English" dataDxfId="10"/>
+    <tableColumn id="1" name="STT" dataDxfId="42"/>
+    <tableColumn id="2" name="ID" dataDxfId="41"/>
+    <tableColumn id="3" name="Text Vietnameses" dataDxfId="40"/>
+    <tableColumn id="4" name="Text English" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:D11" totalsRowShown="0" headerRowDxfId="43" dataDxfId="14" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:D11" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="A5:D11"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="STT" dataDxfId="18"/>
-    <tableColumn id="2" name="ID" dataDxfId="17"/>
-    <tableColumn id="3" name="Text Vietnameses" dataDxfId="16"/>
-    <tableColumn id="4" name="Text English" dataDxfId="15"/>
+    <tableColumn id="1" name="STT" dataDxfId="33"/>
+    <tableColumn id="2" name="ID" dataDxfId="32"/>
+    <tableColumn id="3" name="Text Vietnameses" dataDxfId="31"/>
+    <tableColumn id="4" name="Text English" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A5:D12" totalsRowShown="0" headerRowDxfId="30" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A5:D12" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A5:D12"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="STT" dataDxfId="28"/>
-    <tableColumn id="2" name="ID" dataDxfId="27"/>
-    <tableColumn id="3" name="Text Vietnamese" dataDxfId="26"/>
-    <tableColumn id="4" name="Text English" dataDxfId="25"/>
+    <tableColumn id="1" name="STT" dataDxfId="27"/>
+    <tableColumn id="2" name="ID" dataDxfId="26"/>
+    <tableColumn id="3" name="Text Vietnamese" dataDxfId="25"/>
+    <tableColumn id="4" name="Text English" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A16:D33" totalsRowShown="0" headerRowDxfId="29" dataDxfId="19" headerRowBorderDxfId="32" tableBorderDxfId="33" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A16:D33" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A16:D33"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="STT" dataDxfId="23"/>
-    <tableColumn id="2" name="ID" dataDxfId="22"/>
-    <tableColumn id="4" name="Text Vietnamese" dataDxfId="21"/>
-    <tableColumn id="3" name="Text English" dataDxfId="20"/>
+    <tableColumn id="1" name="STT" dataDxfId="18"/>
+    <tableColumn id="2" name="ID" dataDxfId="17"/>
+    <tableColumn id="4" name="Text Vietnamese" dataDxfId="16"/>
+    <tableColumn id="3" name="Text English" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A6:D15" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A6:D15" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A6:D15"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="STT" dataDxfId="39"/>
-    <tableColumn id="2" name="ID" dataDxfId="38"/>
-    <tableColumn id="3" name="Text Vietnamese" dataDxfId="37"/>
-    <tableColumn id="4" name="Text English" dataDxfId="36"/>
+    <tableColumn id="1" name="STT" dataDxfId="12"/>
+    <tableColumn id="2" name="ID" dataDxfId="11"/>
+    <tableColumn id="3" name="Text Vietnamese" dataDxfId="10"/>
+    <tableColumn id="4" name="Text English" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A7:D13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="2" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A7:D13" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A7:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="STT" dataDxfId="0"/>
-    <tableColumn id="2" name="ID" dataDxfId="1"/>
-    <tableColumn id="3" name="Text Vietnamese" dataDxfId="4"/>
-    <tableColumn id="4" name="Text English" dataDxfId="3"/>
+    <tableColumn id="1" name="STT" dataDxfId="3"/>
+    <tableColumn id="2" name="ID" dataDxfId="2"/>
+    <tableColumn id="3" name="Text Vietnamese" dataDxfId="1"/>
+    <tableColumn id="4" name="Text English" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2166,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,22 +2180,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -2212,128 +2212,128 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24">
+      <c r="A5" s="21">
         <v>1</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
+      <c r="A6" s="34">
         <v>2</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="35" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24">
+      <c r="A7" s="21">
         <v>3</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
+      <c r="A8" s="34">
         <v>4</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="21">
         <v>5</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+      <c r="A10" s="34">
         <v>6</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="35" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
+      <c r="A11" s="21">
         <v>7</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37">
+      <c r="A12" s="34">
         <v>8</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="35" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
+      <c r="A13" s="21">
         <v>9</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2366,22 +2366,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2418,96 +2418,96 @@
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="31">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="32" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40">
+      <c r="A7" s="37">
         <v>2</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="38" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+      <c r="A8" s="31">
         <v>3</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="33" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40">
+      <c r="A9" s="37">
         <v>4</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="38" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
+      <c r="A10" s="31">
         <v>5</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="33" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
+      <c r="A11" s="37">
         <v>6</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="38" t="s">
         <v>55</v>
       </c>
       <c r="E11" s="3"/>
@@ -2548,48 +2548,48 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24">
+      <c r="A15" s="21">
         <v>1</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37">
+      <c r="A16" s="34">
         <v>2</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="36" t="s">
         <v>51</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24">
+      <c r="A17" s="21">
         <v>3</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="23" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="3"/>
@@ -2639,29 +2639,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2691,112 +2691,112 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24">
+      <c r="A6" s="21">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="22" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24">
+      <c r="A7" s="21">
         <v>2</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="23" t="s">
         <v>90</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24">
+      <c r="A8" s="21">
         <v>3</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="23" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="21">
         <v>4</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="23" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24">
+      <c r="A10" s="21">
         <v>5</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="23" t="s">
         <v>61</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
+      <c r="A11" s="21">
         <v>6</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="23" t="s">
         <v>70</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="21">
         <v>7</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="23" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="3"/>
@@ -2811,11 +2811,11 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -2845,13 +2845,13 @@
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
+      <c r="A17" s="24">
         <v>1</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="25" t="s">
         <v>115</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -2861,10 +2861,10 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
+      <c r="A18" s="30">
         <v>2</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="29" t="s">
         <v>113</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -2877,13 +2877,13 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
+      <c r="A19" s="24">
         <v>3</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -2893,13 +2893,13 @@
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
+      <c r="A20" s="30">
         <v>4</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="25" t="s">
         <v>80</v>
       </c>
       <c r="D20" s="14" t="s">
@@ -2909,13 +2909,13 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+      <c r="A21" s="24">
         <v>5</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="25" t="s">
         <v>109</v>
       </c>
       <c r="D21" s="14" t="s">
@@ -2925,13 +2925,13 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33">
+      <c r="A22" s="30">
         <v>6</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="25" t="s">
         <v>82</v>
       </c>
       <c r="D22" s="14" t="s">
@@ -2941,13 +2941,13 @@
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
+      <c r="A23" s="24">
         <v>7</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D23" s="14" t="s">
@@ -2957,13 +2957,13 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="33">
+      <c r="A24" s="30">
         <v>8</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="25" t="s">
         <v>84</v>
       </c>
       <c r="D24" s="14" t="s">
@@ -2973,13 +2973,13 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
+      <c r="A25" s="24">
         <v>9</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="25" t="s">
         <v>88</v>
       </c>
       <c r="D25" s="14" t="s">
@@ -2989,13 +2989,13 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33">
+      <c r="A26" s="30">
         <v>10</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="25" t="s">
         <v>94</v>
       </c>
       <c r="D26" s="14" t="s">
@@ -3005,23 +3005,23 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27">
+      <c r="A27" s="24">
         <v>11</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="26" t="s">
         <v>101</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="33">
+      <c r="A28" s="30">
         <v>12</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -3037,7 +3037,7 @@
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
+      <c r="A29" s="24">
         <v>13</v>
       </c>
       <c r="B29" s="15" t="s">
@@ -3053,7 +3053,7 @@
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33">
+      <c r="A30" s="30">
         <v>14</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -3069,23 +3069,23 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27">
+      <c r="A31" s="24">
         <v>15</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="26" t="s">
         <v>119</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33">
+      <c r="A32" s="30">
         <v>16</v>
       </c>
       <c r="B32" s="15" t="s">
@@ -3101,13 +3101,13 @@
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27">
+      <c r="A33" s="24">
         <v>17</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="28" t="s">
         <v>125</v>
       </c>
       <c r="D33" s="14" t="s">
@@ -3155,22 +3155,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -3181,13 +3181,13 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3199,144 +3199,144 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="20">
         <v>1</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="19" t="s">
         <v>141</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="20">
         <v>2</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="19" t="s">
         <v>140</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="20">
         <v>3</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="19" t="s">
         <v>141</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="20">
         <v>4</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="19" t="s">
         <v>141</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="20">
         <v>5</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>141</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="20">
         <v>6</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="19" t="s">
         <v>141</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="20">
         <v>7</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>141</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+      <c r="A14" s="20">
         <v>8</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="19" t="s">
         <v>139</v>
       </c>
       <c r="E14" s="3"/>
@@ -3366,7 +3366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
@@ -3379,22 +3379,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -3405,13 +3405,13 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3431,112 +3431,112 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47">
+      <c r="A8" s="44">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="47" t="s">
         <v>145</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
+      <c r="A9" s="44">
         <v>2</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="47" t="s">
         <v>151</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="A10" s="44">
         <v>3</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="45" t="s">
         <v>148</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47">
+      <c r="A11" s="44">
         <v>4</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="47" t="s">
         <v>152</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="A12" s="44">
         <v>5</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="47" t="s">
         <v>152</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47">
+      <c r="A13" s="44">
         <v>6</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="49" t="s">
         <v>156</v>
       </c>
       <c r="E13" s="3"/>

</xml_diff>